<commit_message>
New skills for MFJ
</commit_message>
<xml_diff>
--- a/skills/Other Skills.xlsx
+++ b/skills/Other Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kongbinxuan/Desktop/skills-onthology-project/skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009CE333-077A-5F48-B493-6FDE2CB75BF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DE749A-67E3-8C47-B3F5-478269D6BFEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="15080" windowHeight="16180" activeTab="1" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
   </bookViews>
@@ -35,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="163">
   <si>
     <t>Skill</t>
   </si>
   <si>
-    <t>Business</t>
-  </si>
-  <si>
     <t>Support</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>Application</t>
   </si>
   <si>
-    <t>Process</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
@@ -349,9 +343,6 @@
     <t>Subversion</t>
   </si>
   <si>
-    <t>Apahce Subversion</t>
-  </si>
-  <si>
     <t>Tomcat</t>
   </si>
   <si>
@@ -478,12 +469,6 @@
     <t>Google Cloud Platform (GCP)</t>
   </si>
   <si>
-    <t>k-Nearest Neighbours (k-NN)</t>
-  </si>
-  <si>
-    <t>k-Nearest Neighbours (kNN)</t>
-  </si>
-  <si>
     <t>G Suite</t>
   </si>
   <si>
@@ -517,10 +502,28 @@
     <t>Apache Oozie</t>
   </si>
   <si>
-    <t>scikit</t>
-  </si>
-  <si>
-    <t>scikit-learn</t>
+    <t>Apache Subversion</t>
+  </si>
+  <si>
+    <t>k-Nearest Neighbour (kNN)</t>
+  </si>
+  <si>
+    <t>k-Nearest Neighbour (k-NN)</t>
+  </si>
+  <si>
+    <t>Scikit-learn</t>
+  </si>
+  <si>
+    <t>Scikit</t>
+  </si>
+  <si>
+    <t>sklearn</t>
+  </si>
+  <si>
+    <t>Cloud Technologies</t>
+  </si>
+  <si>
+    <t>Cloud Technology</t>
   </si>
 </sst>
 </file>
@@ -594,12 +597,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,10 +622,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCFD10E1-5310-7346-AC41-980E95A43B73}" name="Table1" displayName="Table1" ref="A1:A43" totalsRowShown="0">
-  <autoFilter ref="A1:A43" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A43">
-    <sortCondition ref="A1:A43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCFD10E1-5310-7346-AC41-980E95A43B73}" name="Table1" displayName="Table1" ref="A1:A41" totalsRowShown="0">
+  <autoFilter ref="A1:A41" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A41">
+    <sortCondition ref="A1:A41"/>
   </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{E2BA32DB-C5D4-364B-8EC2-1278FE2E2992}" name="Skill"/>
@@ -631,10 +635,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0EA9FC11-1B29-9647-9CF6-27A3437B58B4}" name="Table13" displayName="Table13" ref="A1:B64" totalsRowShown="0">
-  <autoFilter ref="A1:B64" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B49">
-    <sortCondition ref="B1:B49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0EA9FC11-1B29-9647-9CF6-27A3437B58B4}" name="Table13" displayName="Table13" ref="A1:B66" totalsRowShown="0">
+  <autoFilter ref="A1:B66" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B66">
+    <sortCondition ref="B1:B66"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{55B08FDA-E485-954C-8D9A-ADDF7A1B45A6}" name="Skill"/>
@@ -941,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E914D5-27CD-7E41-A3B3-3B307D4A30A6}">
-  <dimension ref="A1:A43"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -959,52 +963,52 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -1014,157 +1018,147 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1177,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A8B7B5-E1C1-554A-873B-35A5AF2000A8}">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1194,511 +1188,527 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>118</v>
+      <c r="A8" t="s">
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>76</v>
+      <c r="A11" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>88</v>
+      <c r="A16" t="s">
+        <v>140</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>105</v>
+      <c r="A20" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>152</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>151</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>132</v>
+      <c r="A33" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" t="s">
-        <v>65</v>
+        <v>146</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>129</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>128</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>138</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="B53" t="s">
-        <v>140</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>141</v>
+      <c r="A54" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>143</v>
+        <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>144</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="B56" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>150</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>151</v>
-      </c>
-      <c r="B59" s="4" t="s">
         <v>125</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="B61" t="s">
-        <v>155</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="B62" t="s">
-        <v>158</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>159</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>160</v>
       </c>
-      <c r="B64" t="s">
-        <v>161</v>
+      <c r="B66" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix acceltic format skill
</commit_message>
<xml_diff>
--- a/skills/Other Skills.xlsx
+++ b/skills/Other Skills.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kongbinxuan/Desktop/skills-onthology-project/skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DE749A-67E3-8C47-B3F5-478269D6BFEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651D7A77-766D-DB46-8182-93C15AFB0537}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15080" windowHeight="16180" activeTab="1" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
+    <workbookView xWindow="13720" yWindow="460" windowWidth="15080" windowHeight="16180" activeTab="1" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
   </bookViews>
   <sheets>
     <sheet name="Redundant" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="193">
   <si>
     <t>Skill</t>
   </si>
@@ -524,6 +524,96 @@
   </si>
   <si>
     <t>Cloud Technology</t>
+  </si>
+  <si>
+    <t>Visualizations</t>
+  </si>
+  <si>
+    <t>Visualization</t>
+  </si>
+  <si>
+    <t>Dashboards</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence (AI)</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>R Programming</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Mongo DB</t>
+  </si>
+  <si>
+    <t>MongoDB</t>
+  </si>
+  <si>
+    <t>Financial Statements</t>
+  </si>
+  <si>
+    <t>Financial Statement</t>
+  </si>
+  <si>
+    <t>Python Programming</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Reinforcements</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>Data Cleansing/Preparation</t>
+  </si>
+  <si>
+    <t>Data Cleansing</t>
+  </si>
+  <si>
+    <t>Data Storytelling &amp; Presentation Skill</t>
+  </si>
+  <si>
+    <t>Data Storytelling</t>
+  </si>
+  <si>
+    <t>NLP</t>
+  </si>
+  <si>
+    <t>DBMS</t>
+  </si>
+  <si>
+    <t>Regressions</t>
+  </si>
+  <si>
+    <t>ETL</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Structured Query Language (SQL)</t>
+  </si>
+  <si>
+    <t>Natural Language Processing (NLP)</t>
+  </si>
+  <si>
+    <t>Database Management System</t>
+  </si>
+  <si>
+    <t>Extract Transform Load (ETL)</t>
   </si>
 </sst>
 </file>
@@ -635,10 +725,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0EA9FC11-1B29-9647-9CF6-27A3437B58B4}" name="Table13" displayName="Table13" ref="A1:B66" totalsRowShown="0">
-  <autoFilter ref="A1:B66" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B66">
-    <sortCondition ref="B1:B66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0EA9FC11-1B29-9647-9CF6-27A3437B58B4}" name="Table13" displayName="Table13" ref="A1:B81" totalsRowShown="0">
+  <autoFilter ref="A1:B81" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B81">
+    <sortCondition ref="B1:B81"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{55B08FDA-E485-954C-8D9A-ADDF7A1B45A6}" name="Skill"/>
@@ -1171,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A8B7B5-E1C1-554A-873B-35A5AF2000A8}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,290 +1515,410 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>48</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="B39" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" s="4" t="s">
+      <c r="A41" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" t="s">
-        <v>85</v>
+        <v>146</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>165</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>118</v>
+        <v>180</v>
       </c>
       <c r="B46" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
       <c r="B47" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="B50" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>60</v>
+      <c r="A54" t="s">
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>56</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B60" t="s">
-        <v>132</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>94</v>
+      <c r="A61" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>96</v>
-      </c>
-      <c r="B62" t="s">
-        <v>95</v>
+        <v>62</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="B63" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>159</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>158</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>125</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>184</v>
+      </c>
+      <c r="B68" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>176</v>
+      </c>
+      <c r="B70" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>170</v>
+      </c>
+      <c r="B71" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>178</v>
+      </c>
+      <c r="B75" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>119</v>
+      </c>
+      <c r="B77" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>159</v>
+      </c>
+      <c r="B78" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>160</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B79" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>169</v>
+      </c>
+      <c r="B80" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>163</v>
+      </c>
+      <c r="B81" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new skills to database directly
</commit_message>
<xml_diff>
--- a/skills/Other Skills.xlsx
+++ b/skills/Other Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kongbinxuan/Desktop/skills-onthology-project/skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D1D778-BF2B-404C-90D8-95DF4DDE6999}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22062155-82AF-B445-9CD0-F3CAE5440D70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13720" yWindow="460" windowWidth="15080" windowHeight="16180" activeTab="1" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
   </bookViews>
@@ -643,9 +643,6 @@
     <t>Publisher</t>
   </si>
   <si>
-    <t>Microsft Publisher</t>
-  </si>
-  <si>
     <t>Google Colab</t>
   </si>
   <si>
@@ -689,6 +686,9 @@
   </si>
   <si>
     <t>NET</t>
+  </si>
+  <si>
+    <t>Microsoft Publisher</t>
   </si>
 </sst>
 </file>
@@ -801,8 +801,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCFD10E1-5310-7346-AC41-980E95A43B73}" name="Table1" displayName="Table1" ref="A1:A43" totalsRowShown="0">
   <autoFilter ref="A1:A43" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A41">
-    <sortCondition ref="A1:A41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A43">
+    <sortCondition ref="A1:A43"/>
   </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{E2BA32DB-C5D4-364B-8EC2-1278FE2E2992}" name="Skill"/>
@@ -1124,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E914D5-27CD-7E41-A3B3-3B307D4A30A6}">
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1190,162 +1190,162 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>192</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>197</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1360,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A8B7B5-E1C1-554A-873B-35A5AF2000A8}">
   <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" t="s">
         <v>66</v>
@@ -1412,18 +1412,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" t="s">
         <v>213</v>
-      </c>
-      <c r="B6" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" t="s">
         <v>215</v>
-      </c>
-      <c r="B7" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1540,10 +1540,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B22" t="s">
         <v>209</v>
-      </c>
-      <c r="B22" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1668,10 +1668,10 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38" t="s">
         <v>211</v>
-      </c>
-      <c r="B38" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1836,10 +1836,10 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>204</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1852,10 +1852,10 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>202</v>
+      </c>
+      <c r="B61" t="s">
         <v>203</v>
-      </c>
-      <c r="B61" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1887,7 +1887,7 @@
         <v>201</v>
       </c>
       <c r="B65" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2108,10 +2108,10 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B93" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>